<commit_message>
removing excessive data archive
</commit_message>
<xml_diff>
--- a/SacPasRecords/SacPasDailyDataTable2023-09-12.xlsx
+++ b/SacPasRecords/SacPasDailyDataTable2023-09-12.xlsx
@@ -4726,16 +4726,25 @@
         <v>2.42</v>
       </c>
       <c r="O45">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="P45">
-        <v>12908</v>
+        <v>12905</v>
       </c>
       <c r="Q45">
         <v>27.9</v>
       </c>
       <c r="S45">
         <v>24.02</v>
+      </c>
+      <c r="W45">
+        <v>-5520</v>
+      </c>
+      <c r="X45">
+        <v>-5900</v>
+      </c>
+      <c r="Y45">
+        <v>-7280</v>
       </c>
       <c r="Z45">
         <v>6165</v>
@@ -4794,10 +4803,10 @@
         <v>2.5</v>
       </c>
       <c r="O46">
-        <v>2151</v>
+        <v>2146</v>
       </c>
       <c r="P46">
-        <v>12450</v>
+        <v>12445</v>
       </c>
       <c r="Q46">
         <v>28</v>
@@ -4860,6 +4869,15 @@
       </c>
       <c r="M47">
         <v>2.6</v>
+      </c>
+      <c r="O47">
+        <v>2158</v>
+      </c>
+      <c r="P47">
+        <v>12719</v>
+      </c>
+      <c r="Q47">
+        <v>28.3</v>
       </c>
       <c r="R47">
         <v>78</v>

</xml_diff>